<commit_message>
Alex's updated dataset for 7.30.21
</commit_message>
<xml_diff>
--- a/_data/WorldBankGDPData.xlsx
+++ b/_data/WorldBankGDPData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexgenovese/Desktop/R Work/DACSS601/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexgenovese/Desktop/R Work/DACSS601/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC70705A-2333-964A-9CD2-D9361F7E58AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E1B4FD-7D73-4649-94FA-06F5D70609A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="1240" windowWidth="27640" windowHeight="16940" xr2:uid="{8BC6E551-09D9-F446-994B-91770D01FAE9}"/>
+    <workbookView xWindow="15460" yWindow="500" windowWidth="16920" windowHeight="20500" xr2:uid="{8BC6E551-09D9-F446-994B-91770D01FAE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
   <si>
     <t>United States</t>
   </si>
@@ -694,6 +694,9 @@
   </si>
   <si>
     <t>Millions of US Dollars</t>
+  </si>
+  <si>
+    <t>Number of Universities Worldwide in 2020 by Country</t>
   </si>
 </sst>
 </file>
@@ -1057,15 +1060,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5322CA77-5661-8B46-A2F2-06C09BBCFEB8}">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:D218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>217</v>
       </c>
@@ -1075,8 +1078,11 @@
       <c r="C1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1086,8 +1092,11 @@
       <c r="C2">
         <v>20936600</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>3254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1097,8 +1106,11 @@
       <c r="C3">
         <v>14722730.697890099</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1108,8 +1120,11 @@
       <c r="C4">
         <v>5064872.8756045895</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1119,8 +1134,11 @@
       <c r="C5">
         <v>3806060.1401245198</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1130,8 +1148,11 @@
       <c r="C6">
         <v>2707743.7771739103</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1141,8 +1162,11 @@
       <c r="C7">
         <v>2622983.7320064502</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>4381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1152,8 +1176,11 @@
       <c r="C8">
         <v>2603004.3959019501</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1163,8 +1190,11 @@
       <c r="C9">
         <v>1886445.2683407099</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1174,8 +1204,11 @@
       <c r="C10">
         <v>1643407.9770689299</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1185,8 +1218,11 @@
       <c r="C11">
         <v>1630525.0054691101</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1196,8 +1232,11 @@
       <c r="C12">
         <v>1483497.7848676001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1207,8 +1246,11 @@
       <c r="C13">
         <v>1444733.2589716499</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1219,7 +1261,7 @@
         <v>1330900.92505698</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1229,8 +1271,11 @@
       <c r="C15">
         <v>1281199.0910163501</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1240,8 +1285,11 @@
       <c r="C16">
         <v>1076163.31617494</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1251,8 +1299,11 @@
       <c r="C17">
         <v>1058423.83834514</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1263,7 +1314,7 @@
         <v>912242.33511906897</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1274,7 +1325,7 @@
         <v>747968.63617400802</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1285,7 +1336,7 @@
         <v>720101.212394114</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1296,7 +1347,7 @@
         <v>700117.87324926909</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1307,7 +1358,7 @@
         <v>594164.69089493598</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1318,7 +1369,7 @@
         <v>537609.86571901897</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1329,7 +1380,7 @@
         <v>515332.49962786102</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1340,7 +1391,7 @@
         <v>501794.96192524402</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1351,7 +1402,7 @@
         <v>432293.77626239799</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1362,7 +1413,7 @@
         <v>428965.39795945602</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1373,7 +1424,7 @@
         <v>421142.26793737203</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1384,7 +1435,7 @@
         <v>418621.81848230498</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1395,7 +1446,7 @@
         <v>401953.80483708699</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1406,7 +1457,7 @@
         <v>383066.97765356</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>